<commit_message>
SPI Transmit time 37ms -> 10ms
</commit_message>
<xml_diff>
--- a/Drohne/Drohnenprogramme Zeitaufwand.xlsx
+++ b/Drohne/Drohnenprogramme Zeitaufwand.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Arduino code</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Ausgangssituation</t>
+  </si>
+  <si>
+    <t>10ms</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +401,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,15 +412,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -428,7 +437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -438,8 +447,14 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -450,7 +465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -458,12 +473,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>

</xml_diff>